<commit_message>
adjust selfie model to new GSI
</commit_message>
<xml_diff>
--- a/dynamo_modeling.xlsx
+++ b/dynamo_modeling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programas\Maua Dev\selfie_mss_student\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2FD40430-E328-49A9-9740-597CB412B45D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9ECF7C-5FAB-43DE-B3E8-3E906C854EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{9039682F-F14F-4282-9796-110C7624C64A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9039682F-F14F-4282-9796-110C7624C64A}"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
@@ -1026,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{740BCE54-8E19-472E-8D2B-B5BC6C0DF678}">
   <dimension ref="C2:P9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E14:E15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,7 +1037,7 @@
     <col min="5" max="5" width="37.5703125" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" customWidth="1"/>
     <col min="7" max="8" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="39.85546875" customWidth="1"/>
+    <col min="9" max="9" width="45.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
@@ -1250,7 +1250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49426FF8-7284-411E-AA20-16ABF7724AAB}">
   <dimension ref="A2:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>

</xml_diff>